<commit_message>
add testcase create booking VST
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>tc_id</t>
   </si>
@@ -77,7 +77,7 @@
       "agency_player_pay": false,
       "sale_name": "Trần Phương",
       "sale_account": "phuongtt-chilinh",
-      "customer_name": "",
+      "customer_name": "Khách lẻ",
       "caddie_code": "",
       "caddie_booking": "",
       "tee_type": "1",
@@ -110,6 +110,599 @@
   </si>
   <si>
     <t>BB_VST_002</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor with package (package_add_on_fee applied)</t>
+  </si>
+  <si>
+    <t>[
+    {
+      "cms_user": "phuongtt-chilinh",
+      "partner_uid": "CHI-LINH",
+      "course_uid": "CHI-LINH-01",
+      "hole_booking": 18,
+      "customer_booking_name": "PhuongTT",
+      "customer_booking_phone": "",
+      "customer_booking_email": "vn@gmail.com",
+      "agency_id": 0,
+      "booking_restaurant": {
+          "enable": false,
+          "number_people": 0
+      },
+      "booking_retal": {
+          "enable": false,
+          "golf_set_number": 0,
+          "buggy_number": 0
+      },
+      "note_of_booking": "",
+      "agency_player_pay": false,
+      "sale_name": "Trần Phương",
+      "sale_account": "phuongtt-chilinh",
+      "customer_name": "Khách lẻ có package",
+      "caddie_code": "",
+      "caddie_booking": "",
+      "tee_type": "1",
+      "course_type": "A",
+      "tee_path": "NIGHT",
+      "turn_time": "00:34",
+      "tee_time": "22:10",
+      "row_index": 3,
+      "tee_time_after": "",
+      "customer_nationality_id": 3728,
+      "gender": "MALE",
+      "guest_style": "4D_package_PTT",
+      "hole": 18,
+      "booking_date": "{{TODAY}}",
+      "add_ons": [],
+      "voucher_apply": [],
+      "member_uid_of_guest": "",
+      "member_card_uid": ""
+    }
+  ]</t>
+  </si>
+  <si>
+    <t>{
+  "status_code": 200,
+  "size()": 1,
+  "[0].uid": "NOT_NULL",
+  "[0].customer_booking_name": "PhuongTT",
+  "[0].guest_style": "4D_package_PTT"
+}</t>
+  </si>
+  <si>
+    <t>BB_VST_003</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + add caddie</t>
+  </si>
+  <si>
+    <t>[ 
+  {
+      "cms_user": "phuongtt-chilinh",
+      "partner_uid": "CHI-LINH",
+      "course_uid": "CHI-LINH-01",
+      "hole_booking": 18,
+      "customer_booking_name": "PhuongTT",
+      "customer_booking_phone": "",
+      "customer_booking_email": "01zl@gmail.com",
+      "agency_id": 0,
+      "booking_restaurant": {
+          "enable": false,
+          "number_people": 0
+      },
+      "booking_retal": {
+          "enable": false,
+          "golf_set_number": 0,
+          "buggy_number": 0
+      },
+      "note_of_booking": "",
+      "agency_player_pay": false,
+      "sale_name": "Trần Phương",
+      "sale_account": "phuongtt-chilinh",
+      "customer_name": "Khách lẻ booking caddie",
+      "caddie_code": "CD1203",
+      "caddie_booking": "CD1203",
+      "tee_type": "1",
+      "course_type": "A",
+      "tee_path": "NIGHT",
+      "turn_time": "00:42",
+      "tee_time": "22:18",
+      "row_index": 0,
+      "tee_time_after": "",
+      "customer_nationality_id": 3728,
+      "gender": "MALE",
+      "guest_style": "4D",
+      "hole": 18,
+      "booking_date": "{{TODAY}}",
+      "add_ons": [],
+      "voucher_apply": [],
+      "member_uid_of_guest": "",
+      "member_card_uid": ""
+  }
+]</t>
+  </si>
+  <si>
+    <t>{
+  "status_code": 200,
+  "size()": 1,
+  "[0].uid": "NOT_NULL",
+  "[0].has_book_caddie": true
+}</t>
+  </si>
+  <si>
+    <t>BB_VST_004</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor with package + add caddie</t>
+  </si>
+  <si>
+    <t>[
+  {
+      "cms_user": "phuongtt-chilinh",
+      "partner_uid": "CHI-LINH",
+      "course_uid": "CHI-LINH-01",
+      "hole_booking": 18,
+      "customer_booking_name": "PhuongTT",
+      "customer_booking_phone": "",
+      "customer_booking_email": "vn@gmail.com",
+      "agency_id": 0,
+      "booking_restaurant": {
+          "enable": false,
+          "number_people": 0
+      },
+      "booking_retal": {
+          "enable": false,
+          "golf_set_number": 0,
+          "buggy_number": 0
+      },
+      "note_of_booking": "",
+      "agency_player_pay": false,
+      "sale_name": "Trần Phương",
+      "sale_account": "phuongtt-chilinh",
+      "customer_name": "Khách lẻ có package booking caddie",
+      "caddie_code": "009",
+      "caddie_booking": "009",
+      "tee_type": "1",
+      "course_type": "A",
+      "tee_path": "NIGHT",
+      "turn_time": "00:42",
+      "tee_time": "22:18",
+      "row_index": 1,
+      "tee_time_after": "",
+      "customer_nationality_id": 3728,
+      "gender": "MALE",
+      "guest_style": "4D_package_PTT",
+      "hole": 18,
+      "booking_date": "{{TODAY}}",
+      "add_ons": [],
+      "voucher_apply": [],
+      "member_uid_of_guest": "",
+      "member_card_uid": ""
+  }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_005</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (fixed amount, apply to all fee types)</t>
+  </si>
+  <si>
+    <t>[
+  {
+      "cms_user": "phuongtt-chilinh",
+      "partner_uid": "CHI-LINH",
+      "course_uid": "CHI-LINH-01",
+      "hole_booking": 18,
+      "customer_booking_name": "PhuongTT",
+      "customer_booking_phone": "",
+      "customer_booking_email": "vn@gmail.com",
+      "agency_id": 0,
+      "booking_restaurant": {
+          "enable": false,
+          "number_people": 0
+      },
+      "booking_retal": {
+          "enable": false,
+          "golf_set_number": 0,
+          "buggy_number": 0
+      },
+      "note_of_booking": "",
+      "agency_player_pay": false,
+      "sale_name": "Trần Phương",
+      "sale_account": "phuongtt-chilinh",
+      "customer_name": "Khách lẻ VC thông thường",
+      "caddie_code": "",
+      "caddie_booking": "",
+      "tee_type": "1",
+      "course_type": "A",
+      "tee_path": "NIGHT",
+      "turn_time": "00:42",
+      "tee_time": "22:18",
+      "row_index": 2,
+      "tee_time_after": "",
+      "customer_nationality_id": 3728,
+      "gender": "MALE",
+      "guest_style": "4D",
+      "hole": 18,
+      "booking_date": "{{TODAY}}",
+      "add_ons": [],
+      "voucher_apply": [
+          {
+              "id": 23934,
+              "voucher_code": "ATCN0001"
+          }
+      ],
+      "member_uid_of_guest": "",
+      "member_card_uid": ""
+  }
+]</t>
+  </si>
+  <si>
+    <t>{
+  "status_code": 200,
+  "size()": 1,
+  "[0].uid": "NOT_NULL",
+  "[0].customer_booking_name": "PhuongTT",
+  "[0].guest_style": "4D",
+  "[0].IsCheckedIn": false,
+  "[0].bag_status": "BOOKING",
+  "[0].bill_code": "NOT_NULL",
+  "[0].booking_code": "NOT_NULL",
+  "[0].customer_type": "VISITOR",
+  "[0].has_book_caddie": false
+}</t>
+  </si>
+  <si>
+    <t>BB_VST_006</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (fixed amount, apply to green fee only)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "vn@gmail.com",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply normal voucher (fixed amount, apply to green fee only)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:42",
+        "tee_time": "22:18",
+        "row_index": 3,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23936,
+                "voucher_code": "ATGR0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_007</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (fixed amount, apply to caddie fee only)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "vn@gmail.com",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply normal voucher (fixed amount, apply to caddie fee only)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:50",
+        "tee_time": "22:26",
+        "row_index": 0,
+        "tee_time_after": "",
+        "customer_nationality_id": null,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23935,
+                "voucher_code": "ATCD0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_008</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (percent, apply to all fee types)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "vn@gmail.com",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply normal voucher (percent, apply to all fee types)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:50",
+        "tee_time": "22:26",
+        "row_index": 1,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23937,
+                "voucher_code": "ATCN10001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_009</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (percent, apply to green fee only)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "vn@gmail.com",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply normal voucher (percent, apply to green fee only)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:50",
+        "tee_time": "22:26",
+        "row_index": 2,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23938,
+                "voucher_code": "ATGR10001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_010</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply normal voucher (percent, apply to caddie fee only)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "vn@gmail.com",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply normal voucher (percent, apply to caddie fee only)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:50",
+        "tee_time": "22:26",
+        "row_index": 3,
+        "tee_time_after": "",
+        "customer_nationality_id": null,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23939,
+                "voucher_code": "ATCD10001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
+    <t>BB_VST_011</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for 4 fee types: golf/caddie/buggy/add-on package)</t>
+  </si>
+  <si>
+    <t>{"status_code":200}</t>
+  </si>
+  <si>
+    <t>BB_VST_012</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for green fee)</t>
+  </si>
+  <si>
+    <t>BB_VST_013</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for caddie fee)</t>
+  </si>
+  <si>
+    <t>BB_VST_014</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for half buggy)</t>
+  </si>
+  <si>
+    <t>BB_VST_015</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for add-on package)</t>
+  </si>
+  <si>
+    <t>BB_VST_016</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply prepaid voucher (all 4 fee types: golf/caddie/buggy/add-on)</t>
+  </si>
+  <si>
+    <t>BB_VST_017</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply prepaid voucher (green fee only)</t>
+  </si>
+  <si>
+    <t>BB_VST_018</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply prepaid voucher (caddie fee only)</t>
+  </si>
+  <si>
+    <t>BB_VST_019</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply prepaid voucher (half buggy)</t>
+  </si>
+  <si>
+    <t>BB_VST_020</t>
+  </si>
+  <si>
+    <t>Verify create batch booking for Visitor without package + apply prepaid voucher (add-on package)</t>
+  </si>
+  <si>
+    <t>BB_VST_021</t>
   </si>
   <si>
     <t>Verify create batch booking for 2 players successfully</t>
@@ -138,7 +731,7 @@
             "agency_player_pay": false,
             "sale_name": "Trần Phương",
             "sale_account": "phuongtt-chilinh",
-            "customer_name": "",
+            "customer_name": "Player 1",
             "caddie_code": "",
             "caddie_booking": "",
             "tee_type": "1",
@@ -180,7 +773,7 @@
             "agency_player_pay": false,
             "sale_name": "Trần Phương",
             "sale_account": "phuongtt-chilinh",
-            "customer_name": "",
+            "customer_name": "Player 2",
             "caddie_code": "",
             "caddie_booking": "",
             "tee_type": "1",
@@ -211,7 +804,7 @@
 }</t>
   </si>
   <si>
-    <t>BB_VST_003</t>
+    <t>BB_VST_022</t>
   </si>
   <si>
     <t>Verify error when booking_date is missing in player object</t>
@@ -268,7 +861,7 @@
     <t>{"status_code": 500}</t>
   </si>
   <si>
-    <t>BB_VST_004</t>
+    <t>BB_VST_023</t>
   </si>
   <si>
     <t>Verify error when booking date is in the past</t>
@@ -320,7 +913,7 @@
   ]</t>
   </si>
   <si>
-    <t>BB_VST_005</t>
+    <t>BB_VST_024</t>
   </si>
   <si>
     <t>Verify error when guest_style is invalid</t>
@@ -372,272 +965,6 @@
   ]</t>
   </si>
   <si>
-    <t>BB_VST_006</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor with package (package_add_on_fee applied)</t>
-  </si>
-  <si>
-    <t>{
-    "booking_list": [
-        {
-            "cms_user": "phuongtt-chilinh",
-            "partner_uid": "CHI-LINH",
-            "course_uid": "CHI-LINH-01",
-            "hole_booking": 18,
-            "customer_booking_name": "PhuongTT",
-            "customer_booking_phone": "",
-            "customer_booking_email": "vn@gmail.com",
-            "agency_id": 0,
-            "booking_restaurant": {
-                "enable": false,
-                "number_people": 0
-            },
-            "booking_retal": {
-                "enable": false,
-                "golf_set_number": 0,
-                "buggy_number": 0
-            },
-            "note_of_booking": "",
-            "agency_player_pay": false,
-            "sale_name": "Trần Phương",
-            "sale_account": "phuongtt-chilinh",
-            "customer_name": "",
-            "caddie_code": "",
-            "caddie_booking": "",
-            "tee_type": "1",
-            "course_type": "A",
-            "tee_path": "NIGHT",
-            "turn_time": "00:34",
-            "tee_time": "22:10",
-            "row_index": 3,
-            "tee_time_after": "",
-            "customer_nationality_id": 3728,
-            "gender": "MALE",
-            "guest_style": "4D_package_PTT",
-            "hole": 18,
-            "booking_date": "{{TODAY}}",
-            "add_ons": [],
-            "voucher_apply": [],
-            "member_uid_of_guest": "",
-            "member_card_uid": ""
-        }
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  "status_code": 200,
-  "size()": 1,
-  "[0].uid": "NOT_NULL"
-}</t>
-  </si>
-  <si>
-    <t>BB_VST_007</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + add caddie</t>
-  </si>
-  <si>
-    <t>{
-    "booking_list": [
-        {
-            "cms_user": "phuongtt-chilinh",
-            "partner_uid": "CHI-LINH",
-            "course_uid": "CHI-LINH-01",
-            "hole_booking": 18,
-            "customer_booking_name": "PhuongTT",
-            "customer_booking_phone": "",
-            "customer_booking_email": "01zl@gmail.com",
-            "agency_id": 0,
-            "booking_restaurant": {
-                "enable": false,
-                "number_people": 0
-            },
-            "booking_retal": {
-                "enable": false,
-                "golf_set_number": 0,
-                "buggy_number": 0
-            },
-            "note_of_booking": "",
-            "agency_player_pay": false,
-            "sale_name": "Trần Phương",
-            "sale_account": "phuongtt-chilinh",
-            "customer_name": "",
-            "caddie_code": "CD1203",
-            "caddie_booking": "CD1203",
-            "tee_type": "1",
-            "course_type": "A",
-            "tee_path": "NIGHT",
-            "turn_time": "00:42",
-            "tee_time": "22:18",
-            "row_index": 0,
-            "tee_time_after": "",
-            "customer_nationality_id": 3728,
-            "gender": "MALE",
-            "guest_style": "4D",
-            "hole": 18,
-            "booking_date": "{{TODAY}}",
-            "add_ons": [],
-            "voucher_apply": [],
-            "member_uid_of_guest": "",
-            "member_card_uid": ""
-        }
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{
-  "status_code": 200,
-  "size()": 1,
-  "[0].uid": "NOT_NULL",
-}</t>
-  </si>
-  <si>
-    <t>BB_VST_008</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor with package + add caddie</t>
-  </si>
-  <si>
-    <t>{
-    "booking_list": [
-        {
-            "cms_user": "phuongtt-chilinh",
-            "partner_uid": "CHI-LINH",
-            "course_uid": "CHI-LINH-01",
-            "hole_booking": 18,
-            "customer_booking_name": "PhuongTT",
-            "customer_booking_phone": "",
-            "customer_booking_email": "vn@gmail.com",
-            "agency_id": 0,
-            "booking_restaurant": {
-                "enable": false,
-                "number_people": 0
-            },
-            "booking_retal": {
-                "enable": false,
-                "golf_set_number": 0,
-                "buggy_number": 0
-            },
-            "note_of_booking": "",
-            "agency_player_pay": false,
-            "sale_name": "Trần Phương",
-            "sale_account": "phuongtt-chilinh",
-            "customer_name": "",
-            "caddie_code": "009",
-            "caddie_booking": "009",
-            "tee_type": "1",
-            "course_type": "A",
-            "tee_path": "NIGHT",
-            "turn_time": "00:42",
-            "tee_time": "22:18",
-            "row_index": 1,
-            "tee_time_after": "",
-            "customer_nationality_id": 3728,
-            "gender": "MALE",
-            "guest_style": "4D_package_PTT",
-            "hole": 18,
-            "booking_date": "{{TODAY}}",
-            "add_ons": [],
-            "voucher_apply": [],
-            "member_uid_of_guest": "",
-            "member_card_uid": ""
-        }
-    ]
-}</t>
-  </si>
-  <si>
-    <t>BB_VST_009</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed amount, apply to all fee types)</t>
-  </si>
-  <si>
-    <t>{"status_code":200,"[0].voucher_apply[0].voucher_code":"{{VOUCHER_ALL_FIXED}}","[0].total_amount":"NOT_NULL"}</t>
-  </si>
-  <si>
-    <t>BB_VST_010</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed amount, apply to green fee only)</t>
-  </si>
-  <si>
-    <t>{"status_code":200,"[0].voucher_apply[0].voucher_code":"{{VOUCHER_GREEN_FIXED}}"}</t>
-  </si>
-  <si>
-    <t>BB_VST_011</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed amount, apply to caddie fee only)</t>
-  </si>
-  <si>
-    <t>{"status_code":200,"[0].voucher_apply[0].voucher_code":"{{VOUCHER_CADDIE_FIXED}}"}</t>
-  </si>
-  <si>
-    <t>BB_VST_012</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (percent, apply to all fee types)</t>
-  </si>
-  <si>
-    <t>{"status_code":200,"[0].voucher_apply[0].voucher_code":"{{VOUCHER_ALL_PERCENT}}"}</t>
-  </si>
-  <si>
-    <t>BB_VST_013</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (percent, apply to green fee only)</t>
-  </si>
-  <si>
-    <t>{"status_code":200,"[0].voucher_apply[0].voucher_code":"{{VOUCHER_GREEN_PERCENT}}"}</t>
-  </si>
-  <si>
-    <t>BB_VST_014</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (percent, apply to caddie fee only)</t>
-  </si>
-  <si>
-    <t>{"status_code":200}</t>
-  </si>
-  <si>
-    <t>BB_VST_015</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed discount for 4 fee types: golf/caddie/buggy/add-on)</t>
-  </si>
-  <si>
-    <t>BB_VST_016</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed discount for green fee)</t>
-  </si>
-  <si>
-    <t>BB_VST_017</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed discount for caddie fee)</t>
-  </si>
-  <si>
-    <t>BB_VST_018</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed discount for half buggy)</t>
-  </si>
-  <si>
-    <t>BB_VST_019</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor without package + voucher (fixed discount for add-on package)</t>
-  </si>
-  <si>
-    <t>BB_VST_020</t>
-  </si>
-  <si>
-    <t>Verify create batch booking for Visitor with package + voucher (percent, apply to all fee types)</t>
-  </si>
-  <si>
     <t>BB_001</t>
   </si>
   <si>
@@ -668,6 +995,9 @@
     <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường / Trực tiếp số tiền / Áp dụng tất cả các loại phí</t>
   </si>
   <si>
+    <t>VC còn các case giảm về 0đ</t>
+  </si>
+  <si>
     <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường / Trực tiếp số tiền / Áp dụng chỉ green fee</t>
   </si>
   <si>
@@ -696,6 +1026,21 @@
   </si>
   <si>
     <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / Add-on package</t>
+  </si>
+  <si>
+    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Cho 4 loại phí</t>
+  </si>
+  <si>
+    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Green fee</t>
+  </si>
+  <si>
+    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Caddie fee</t>
+  </si>
+  <si>
+    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / 1/2 xe</t>
+  </si>
+  <si>
+    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Add-on package</t>
   </si>
 </sst>
 </file>
@@ -874,7 +1219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -895,6 +1240,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1074,7 +1425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1133,66 +1484,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1320,7 +1611,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1332,119 +1623,119 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1469,35 +1760,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2032,353 +2332,425 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" style="8" customWidth="1"/>
-    <col min="2" max="2" width="54.1428571428571" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" style="8" customWidth="1"/>
-    <col min="4" max="4" width="59.8571428571429" style="8" customWidth="1"/>
-    <col min="5" max="5" width="37.1428571428571" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.14285714285714" style="8"/>
+    <col min="1" max="1" width="13.1428571428571" style="9" customWidth="1"/>
+    <col min="2" max="2" width="115.285714285714" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.8571428571429" style="9" customWidth="1"/>
+    <col min="4" max="4" width="59.8571428571429" style="9" customWidth="1"/>
+    <col min="5" max="5" width="37.1428571428571" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.14285714285714" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" customHeight="1" spans="1:5">
-      <c r="A1" s="9" t="s">
+    <row r="1" ht="63" customHeight="1" spans="1:5">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="148" customHeight="1" spans="1:5">
-      <c r="A2" s="13" t="s">
+    <row r="2" ht="63" customHeight="1" spans="1:5">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" ht="80" customHeight="1" spans="1:5">
-      <c r="A3" s="13" t="s">
+    <row r="3" ht="63" customHeight="1" spans="1:5">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="65" customHeight="1" spans="1:5">
-      <c r="A4" s="13" t="s">
+    <row r="4" ht="63" customHeight="1" spans="1:5">
+      <c r="A4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="13" t="s">
+    </row>
+    <row r="5" ht="63" customHeight="1" spans="1:5">
+      <c r="A5" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" ht="78" customHeight="1" spans="1:5">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="E5" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" ht="63" customHeight="1" spans="1:5">
+      <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" ht="63" customHeight="1" spans="1:5">
-      <c r="A6" s="13" t="s">
+      <c r="B6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="E6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" ht="111" customHeight="1" spans="1:5">
-      <c r="A7" s="13" t="s">
+    </row>
+    <row r="7" ht="63" customHeight="1" spans="1:5">
+      <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" ht="63" customHeight="1" spans="1:5">
+      <c r="A8" s="14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" ht="141" customHeight="1" spans="1:5">
-      <c r="A8" s="13" t="s">
+      <c r="B8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" ht="63" customHeight="1" spans="1:5">
+      <c r="A9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="140" customHeight="1" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="D9" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" ht="63" customHeight="1" spans="1:5">
+      <c r="A10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="B10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" ht="45" spans="1:5">
-      <c r="A10" s="13" t="s">
+      <c r="D10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" ht="63" customHeight="1" spans="1:5">
+      <c r="A11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" ht="45" spans="1:5">
-      <c r="A11" s="13" t="s">
+      <c r="D11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" ht="63" customHeight="1" spans="1:5">
+      <c r="A12" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" ht="45" spans="1:5">
-      <c r="A12" s="13" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="1" t="s">
+    </row>
+    <row r="13" ht="63" customHeight="1" spans="1:5">
+      <c r="A13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" ht="45" spans="1:5">
-      <c r="A13" s="13" t="s">
+      <c r="D13" s="18"/>
+      <c r="E13" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" ht="63" customHeight="1" spans="1:5">
+      <c r="A14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="D14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" ht="63" customHeight="1" spans="1:5">
+      <c r="A15" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" ht="45" spans="1:5">
-      <c r="A14" s="13" t="s">
+      <c r="B15" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" ht="63" customHeight="1" spans="1:5">
+      <c r="A16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B16" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" ht="30" spans="1:5">
-      <c r="A15" s="13" t="s">
+      <c r="D16" s="18"/>
+      <c r="E16" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" ht="63" customHeight="1" spans="1:5">
+      <c r="A17" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" ht="63" customHeight="1" spans="1:5">
+      <c r="A18" s="14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" ht="45" spans="1:5">
-      <c r="A16" s="13" t="s">
+      <c r="B18" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C18" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" ht="63" customHeight="1" spans="1:5">
+      <c r="A19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="B19" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" ht="30" spans="1:5">
-      <c r="A17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" ht="63" customHeight="1" spans="1:5">
+      <c r="A20" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="B20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" ht="30" spans="1:5">
-      <c r="A18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="1" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" ht="63" customHeight="1" spans="1:5">
+      <c r="A21" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" ht="30" spans="1:5">
-      <c r="A19" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" ht="63" customHeight="1" spans="1:5">
+      <c r="A22" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B22" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" ht="30" spans="1:5">
-      <c r="A20" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="D22" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" ht="30" spans="1:5">
-      <c r="A21" s="13" t="s">
+      <c r="E22" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="23" ht="63" customHeight="1" spans="1:5">
+      <c r="A23" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
+      <c r="B23" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" ht="63" customHeight="1" spans="1:5">
+      <c r="A24" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" ht="63" customHeight="1" spans="1:5">
+      <c r="A25" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2390,10 +2762,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2425,10 +2797,10 @@
     </row>
     <row r="2" ht="77" customHeight="1" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2436,10 +2808,10 @@
     </row>
     <row r="3" ht="96" customHeight="1" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -2447,10 +2819,10 @@
     </row>
     <row r="4" ht="110" customHeight="1" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -2458,10 +2830,10 @@
     </row>
     <row r="5" ht="113" customHeight="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -2469,63 +2841,90 @@
     </row>
     <row r="6" ht="82" customHeight="1" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" ht="45" spans="2:2">
-      <c r="B7" s="6" t="s">
-        <v>76</v>
+      <c r="B7" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" ht="45" spans="2:2">
-      <c r="B8" s="6" t="s">
-        <v>77</v>
+      <c r="B8" s="8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" ht="45" spans="2:2">
-      <c r="B9" s="6" t="s">
-        <v>78</v>
+      <c r="B9" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="10" ht="45" spans="2:2">
-      <c r="B10" s="6" t="s">
-        <v>79</v>
+      <c r="B10" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" ht="45" spans="2:2">
-      <c r="B11" s="6" t="s">
-        <v>80</v>
+      <c r="B11" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="12" ht="30" spans="2:2">
       <c r="B12" s="6" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" ht="30" spans="2:2">
       <c r="B13" s="6" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:2">
       <c r="B14" s="6" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" ht="30" spans="2:2">
       <c r="B15" s="6" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" ht="30" spans="2:2">
       <c r="B16" s="6" t="s">
-        <v>85</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" ht="30" spans="2:2">
+      <c r="B17" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" ht="30" spans="2:2">
+      <c r="B18" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="2:2">
+      <c r="B19" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" ht="30" spans="2:2">
+      <c r="B20" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" ht="30" spans="2:2">
+      <c r="B21" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create integration booking price
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11460"/>
+    <workbookView windowWidth="30240" windowHeight="13080"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
   <si>
     <t>tc_id</t>
   </si>
@@ -645,7 +645,55 @@
     <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for 4 fee types: golf/caddie/buggy/add-on package)</t>
   </si>
   <si>
-    <t>{"status_code":200}</t>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply fixed discount voucher (fixed discount for 4 fee types: golf/caddie/buggy/add-on package)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:58",
+        "tee_time": "22:34",
+        "row_index": 0,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23941,
+                "voucher_code": "AT4FEE0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
   </si>
   <si>
     <t>BB_VST_012</t>
@@ -654,52 +702,511 @@
     <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for green fee)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply fixed discount voucher (fixed discount for green fee)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:58",
+        "tee_time": "22:34",
+        "row_index": 1,
+        "tee_time_after": "",
+        "customer_nationality_id": null,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23942,
+                "voucher_code": "AT4GR0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_013</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for caddie fee)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply fixed discount voucher (fixed discount for caddie fee)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:58",
+        "tee_time": "22:34",
+        "row_index": 2,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23943,
+                "voucher_code": "AT4CD0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_014</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for half buggy)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply fixed discount voucher (fixed discount for half buggy)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "00:58",
+        "tee_time": "22:34",
+        "row_index": 3,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23944,
+                "voucher_code": "AT4BG0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_015</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply fixed discount voucher (fixed discount for add-on package)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply fixed discount voucher (fixed discount for add-on package)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "01:06",
+        "tee_time": "22:42",
+        "row_index": 0,
+        "tee_time_after": "",
+        "customer_nationality_id": null,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23945,
+                "voucher_code": "AT4PACKAGE0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_016</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply prepaid voucher (all 4 fee types: golf/caddie/buggy/add-on)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply prepaid voucher (all 4 fee types: golf/caddie/buggy/add-on)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "01:06",
+        "tee_time": "22:42",
+        "row_index": 1,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23947,
+                "voucher_code": "ATTC4FREE0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_017</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply prepaid voucher (green fee only)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply prepaid voucher (green fee only)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "01:06",
+        "tee_time": "22:42",
+        "row_index": 2,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23948,
+                "voucher_code": "ATTC4GR0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_018</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply prepaid voucher (caddie fee only)</t>
   </si>
   <si>
+    <t>[
+        {
+            "cms_user": "phuongtt-chilinh",
+            "partner_uid": "CHI-LINH",
+            "course_uid": "CHI-LINH-01",
+            "hole_booking": 18,
+            "customer_booking_name": "PhuongTT",
+            "customer_booking_phone": "",
+            "customer_booking_email": "phuongtt@caro.vn",
+            "agency_id": 0,
+            "booking_restaurant": {
+                "enable": false,
+                "number_people": 0
+            },
+            "booking_retal": {
+                "enable": false,
+                "golf_set_number": 0,
+                "buggy_number": 0
+            },
+            "note_of_booking": "",
+            "agency_player_pay": false,
+            "sale_name": "Trần Phương",
+            "sale_account": "phuongtt-chilinh",
+            "customer_name": "VST apply prepaid voucher (caddie fee only)",
+            "caddie_code": "",
+            "caddie_booking": "",
+            "tee_type": "1",
+            "course_type": "A",
+            "tee_path": "NIGHT",
+            "turn_time": "01:06",
+            "tee_time": "22:42",
+            "row_index": 3,
+            "tee_time_after": "",
+            "customer_nationality_id": 3728,
+            "gender": "MALE",
+            "guest_style": "4D",
+            "hole": 18,
+            "booking_date": "{{TODAY}}",
+            "add_ons": [],
+            "voucher_apply": [
+                {
+                    "id": 23949,
+                    "voucher_code": "ATTC4CD0001"
+                }
+            ],
+            "member_uid_of_guest": "",
+            "member_card_uid": ""
+        }
+    ]</t>
+  </si>
+  <si>
     <t>BB_VST_019</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply prepaid voucher (half buggy)</t>
   </si>
   <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply prepaid voucher (half buggy)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "01:14",
+        "tee_time": "22:50",
+        "row_index": 0,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23950,
+                "voucher_code": "ATTC4BG0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
+  </si>
+  <si>
     <t>BB_VST_020</t>
   </si>
   <si>
     <t>Verify create batch booking for Visitor without package + apply prepaid voucher (add-on package)</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "cms_user": "phuongtt-chilinh",
+        "partner_uid": "CHI-LINH",
+        "course_uid": "CHI-LINH-01",
+        "hole_booking": 18,
+        "customer_booking_name": "PhuongTT",
+        "customer_booking_phone": "",
+        "customer_booking_email": "phuongtt@caro.vn",
+        "agency_id": 0,
+        "booking_restaurant": {
+            "enable": false,
+            "number_people": 0
+        },
+        "booking_retal": {
+            "enable": false,
+            "golf_set_number": 0,
+            "buggy_number": 0
+        },
+        "note_of_booking": "",
+        "agency_player_pay": false,
+        "sale_name": "Trần Phương",
+        "sale_account": "phuongtt-chilinh",
+        "customer_name": "VST apply prepaid voucher (add-on package)",
+        "caddie_code": "",
+        "caddie_booking": "",
+        "tee_type": "1",
+        "course_type": "A",
+        "tee_path": "NIGHT",
+        "turn_time": "01:14",
+        "tee_time": "22:50",
+        "row_index": 1,
+        "tee_time_after": "",
+        "customer_nationality_id": 3728,
+        "gender": "MALE",
+        "guest_style": "4D",
+        "hole": 18,
+        "booking_date": "{{TODAY}}",
+        "add_ons": [],
+        "voucher_apply": [
+            {
+                "id": 23951,
+                "voucher_code": "ATTC4PACKAGE0001"
+            }
+        ],
+        "member_uid_of_guest": "",
+        "member_card_uid": ""
+    }
+]</t>
   </si>
   <si>
     <t>BB_VST_021</t>
@@ -1048,10 +1555,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1593,16 +2100,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1735,7 +2242,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1751,18 +2258,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1775,29 +2282,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2334,18 +2832,18 @@
   <sheetPr/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B19" sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" style="9" customWidth="1"/>
-    <col min="2" max="2" width="115.285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.8571428571429" style="9" customWidth="1"/>
-    <col min="4" max="4" width="59.8571428571429" style="9" customWidth="1"/>
-    <col min="5" max="5" width="37.1428571428571" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.14285714285714" style="9"/>
+    <col min="1" max="1" width="13.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="115.2890625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.859375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="59.859375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="63" customHeight="1" spans="1:5">
@@ -2361,396 +2859,416 @@
       <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="63" customHeight="1" spans="1:5">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="63" customHeight="1" spans="1:5">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" ht="63" customHeight="1" spans="1:5">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" ht="63" customHeight="1" spans="1:5">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="63" customHeight="1" spans="1:5">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="63" customHeight="1" spans="1:5">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" ht="63" customHeight="1" spans="1:5">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" ht="63" customHeight="1" spans="1:5">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="63" customHeight="1" spans="1:5">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" ht="63" customHeight="1" spans="1:5">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" ht="63" customHeight="1" spans="1:5">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="15" t="s">
         <v>42</v>
       </c>
+      <c r="E12" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" ht="63" customHeight="1" spans="1:5">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18" t="s">
-        <v>42</v>
+      <c r="D13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" ht="63" customHeight="1" spans="1:5">
-      <c r="A14" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="A14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
-        <v>42</v>
+      <c r="D14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" ht="63" customHeight="1" spans="1:5">
-      <c r="A15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="A15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18" t="s">
-        <v>42</v>
+      <c r="D15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" ht="63" customHeight="1" spans="1:5">
-      <c r="A16" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="18" t="s">
+      <c r="A16" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
-        <v>42</v>
+      <c r="D16" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="63" customHeight="1" spans="1:5">
-      <c r="A17" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="A17" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="18" t="s">
-        <v>42</v>
+      <c r="D17" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="18" ht="63" customHeight="1" spans="1:5">
-      <c r="A18" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="18" t="s">
+      <c r="A18" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="18" t="s">
-        <v>42</v>
+      <c r="D18" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" ht="63" customHeight="1" spans="1:5">
-      <c r="A19" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="A19" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="18" t="s">
-        <v>42</v>
+      <c r="D19" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" ht="63" customHeight="1" spans="1:5">
-      <c r="A20" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="18" t="s">
+      <c r="A20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="18" t="s">
-        <v>42</v>
+      <c r="D20" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" ht="63" customHeight="1" spans="1:5">
-      <c r="A21" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="18" t="s">
+      <c r="A21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="18" t="s">
-        <v>42</v>
+      <c r="D21" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" ht="63" customHeight="1" spans="1:5">
-      <c r="A22" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="A22" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>64</v>
+      <c r="D22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="23" ht="63" customHeight="1" spans="1:5">
-      <c r="A23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>69</v>
+      <c r="A23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="24" ht="63" customHeight="1" spans="1:5">
-      <c r="A24" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>69</v>
+      <c r="A24" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" ht="63" customHeight="1" spans="1:5">
-      <c r="A25" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>69</v>
+      <c r="A25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2768,17 +3286,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="1"/>
-    <col min="2" max="2" width="49.7142857142857" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.8571428571429" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.1428571428571" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5714285714286" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.14285714285714" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="49.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.859375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="73.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:5">
+    <row r="1" ht="21" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2791,140 +3309,140 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="77" customHeight="1" spans="1:5">
-      <c r="A2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" ht="96" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" ht="110" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" ht="113" customHeight="1" spans="1:5">
-      <c r="A5" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" ht="82" customHeight="1" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" ht="45" spans="2:2">
-      <c r="B7" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" ht="45" spans="2:2">
-      <c r="B8" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" ht="45" spans="2:2">
-      <c r="B9" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" ht="45" spans="2:2">
-      <c r="B10" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" ht="45" spans="2:2">
-      <c r="B11" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" ht="30" spans="2:2">
-      <c r="B12" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" ht="30" spans="2:2">
-      <c r="B13" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14" ht="30" spans="2:2">
-      <c r="B14" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" ht="30" spans="2:2">
-      <c r="B15" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" ht="30" spans="2:2">
-      <c r="B16" s="6" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" ht="51" spans="2:2">
+      <c r="B7" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" ht="30" spans="2:2">
-      <c r="B17" s="8" t="s">
+    <row r="8" ht="51" spans="2:2">
+      <c r="B8" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" ht="30" spans="2:2">
-      <c r="B18" s="8" t="s">
+    <row r="9" ht="51" spans="2:2">
+      <c r="B9" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" ht="30" spans="2:2">
-      <c r="B19" s="8" t="s">
+    <row r="10" ht="34" spans="2:2">
+      <c r="B10" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" ht="30" spans="2:2">
-      <c r="B20" s="8" t="s">
+    <row r="11" ht="34" spans="2:2">
+      <c r="B11" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="21" ht="30" spans="2:2">
-      <c r="B21" s="8" t="s">
+    <row r="12" ht="34" spans="2:2">
+      <c r="B12" s="5" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="13" ht="34" spans="2:2">
+      <c r="B13" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" ht="34" spans="2:2">
+      <c r="B14" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" ht="34" spans="2:2">
+      <c r="B15" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" ht="34" spans="2:2">
+      <c r="B16" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" ht="34" spans="2:2">
+      <c r="B17" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" ht="34" spans="2:2">
+      <c r="B18" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" ht="34" spans="2:2">
+      <c r="B19" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" ht="34" spans="2:2">
+      <c r="B20" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" ht="34" spans="2:2">
+      <c r="B21" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel create booking
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13080"/>
+    <workbookView windowWidth="30240" windowHeight="12480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="input_data" sheetId="4" r:id="rId2"/>
+    <sheet name="expected_data" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="145">
   <si>
     <t>tc_id</t>
   </si>
@@ -1472,82 +1473,184 @@
   ]</t>
   </si>
   <si>
-    <t>BB_001</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package</t>
-  </si>
-  <si>
-    <t>BB_002</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee có package</t>
-  </si>
-  <si>
-    <t>BB_003</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + add thêm caddie</t>
-  </si>
-  <si>
-    <t>BB_004</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee có package + add thêm caddie</t>
-  </si>
-  <si>
-    <t>BB_005</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường / Trực tiếp số tiền / Áp dụng tất cả các loại phí</t>
-  </si>
-  <si>
-    <t>VC còn các case giảm về 0đ</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường / Trực tiếp số tiền / Áp dụng chỉ green fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường / Trực tiếp số tiền / Áp dụng chỉ caddie</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường /  % vào giá / Áp dụng tất cả các loại phí</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường /  % vào giá / Áp dụng chỉ green fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá thông thường /  % vào giá / Áp dụng chỉ caddie</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / Cho 4 loại phí</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / Green fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / Caddie fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / 1/2 xe</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC giảm giá cố định / Add-on package</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Cho 4 loại phí</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Green fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Caddie fee</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / 1/2 xe</t>
-  </si>
-  <si>
-    <t>VST_Kiểm ra booking golf fee không có package + Apply VC trả trước / Add-on package</t>
+    <t>key</t>
+  </si>
+  <si>
+    <t>value_case1</t>
+  </si>
+  <si>
+    <t>value_case2</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    "booking_list": [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "cms_user": ,</t>
+  </si>
+  <si>
+    <t>"phuongtt-chilinh01"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "partner_uid": ,</t>
+  </si>
+  <si>
+    <t>"CHI-LINH"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "course_uid": ,</t>
+  </si>
+  <si>
+    <t>"CHI-LINH-01"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "hole_booking": ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_booking_name": ,</t>
+  </si>
+  <si>
+    <t>"PhuongTT"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_booking_phone": ,</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_booking_email": "phuongtt@caro.vn",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "agency_id": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "booking_restaurant": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "enable": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "number_people": 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "booking_retal": {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "golf_set_number": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                "buggy_number": 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "note_of_booking": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "agency_player_pay": false,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "sale_name": "Trần Phương 01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "sale_account": "phuongtt-chilinh01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_name": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "caddie_code": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "caddie_booking": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "tee_type": "1",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "course_type": "A",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "tee_path": "NOON",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "turn_time": "17:56",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "tee_time": "15:32",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "row_index": 0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "tee_time_after": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_nationality_id": 3728,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "gender": "MALE",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "guest_style": "4D",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "hole": 18,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "booking_date": "08/09/2025",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "add_ons": [],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "voucher_apply": [],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "member_uid_of_guest": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "member_card_uid": ""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "cms_user": "phuongtt-chilinh01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "partner_uid": "CHI-LINH",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "course_uid": "CHI-LINH-01",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "hole_booking": 18,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_booking_name": "PhuongTT",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "customer_booking_phone": "",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            "row_index": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ]</t>
+  </si>
+  <si>
+    <t>}</t>
   </si>
 </sst>
 </file>
@@ -1932,50 +2035,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2118,7 +2182,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2130,34 +2194,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2242,59 +2306,47 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2832,442 +2884,443 @@
   <sheetPr/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B19" sqref="A1:E25"/>
+    <sheetView zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="115.2890625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.859375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="59.859375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="9"/>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="115.2890625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.859375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.859375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.9765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.3203125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="63" customHeight="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="63" customHeight="1" spans="1:5">
-      <c r="A2" s="13" t="s">
+    <row r="2" ht="163" customHeight="1" spans="1:5">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="63" customHeight="1" spans="1:5">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" ht="63" customHeight="1" spans="1:5">
-      <c r="A4" s="13" t="s">
+    <row r="4" ht="139" customHeight="1" spans="1:5">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" ht="63" customHeight="1" spans="1:5">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" ht="63" customHeight="1" spans="1:5">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" ht="63" customHeight="1" spans="1:5">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" ht="63" customHeight="1" spans="1:5">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" ht="63" customHeight="1" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" ht="63" customHeight="1" spans="1:5">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" ht="63" customHeight="1" spans="1:5">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" ht="63" customHeight="1" spans="1:5">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" ht="63" customHeight="1" spans="1:5">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" ht="63" customHeight="1" spans="1:5">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" ht="63" customHeight="1" spans="1:5">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" ht="63" customHeight="1" spans="1:5">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" ht="63" customHeight="1" spans="1:5">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" ht="63" customHeight="1" spans="1:5">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" ht="63" customHeight="1" spans="1:5">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" ht="63" customHeight="1" spans="1:5">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" ht="63" customHeight="1" spans="1:5">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" ht="63" customHeight="1" spans="1:5">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="12" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="23" ht="63" customHeight="1" spans="1:5">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" ht="63" customHeight="1" spans="1:5">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" ht="63" customHeight="1" spans="1:5">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3280,173 +3333,506 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="49.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.859375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="73.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="48.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="49.0859375" customWidth="1"/>
+    <col min="2" max="2" width="18.4765625" customWidth="1"/>
+    <col min="3" max="3" width="13.8046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" ht="77" customHeight="1" spans="1:5">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B1" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" ht="96" customHeight="1" spans="1:5">
-      <c r="A3" s="5" t="s">
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" ht="110" customHeight="1" spans="1:5">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="5" t="s">
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" ht="113" customHeight="1" spans="1:5">
-      <c r="A5" s="5" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" ht="82" customHeight="1" spans="1:5">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="5" t="s">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" ht="51" spans="2:2">
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="8" ht="51" spans="2:2">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" ht="51" spans="2:2">
-      <c r="B9" s="7" t="s">
+      <c r="B8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" ht="34" spans="2:2">
-      <c r="B10" s="7" t="s">
+      <c r="B9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" ht="34" spans="2:2">
-      <c r="B11" s="7" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" ht="34" spans="2:2">
-      <c r="B12" s="5" t="s">
+      <c r="B10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" ht="34" spans="2:2">
-      <c r="B13" s="5" t="s">
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" ht="34" spans="2:2">
-      <c r="B14" s="5" t="s">
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" ht="34" spans="2:2">
-      <c r="B15" s="5" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" ht="34" spans="2:2">
-      <c r="B16" s="5" t="s">
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" ht="34" spans="2:2">
-      <c r="B17" s="7" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" ht="34" spans="2:2">
-      <c r="B18" s="7" t="s">
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" ht="34" spans="2:2">
-      <c r="B19" s="7" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" ht="34" spans="2:2">
-      <c r="B20" s="7" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" ht="34" spans="2:2">
-      <c r="B21" s="7" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update create booking batch
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13100"/>
+    <workbookView windowWidth="28800" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="191">
   <si>
     <t>tc_id</t>
   </si>
@@ -303,9 +303,6 @@
     <t>22:18</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>BB_VST_004</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
   </si>
   <si>
     <t>failed</t>
+  </si>
+  <si>
+    <t>create_booking_batch_error_expect.json</t>
   </si>
   <si>
     <t>BB_VST_022</t>
@@ -637,10 +637,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1196,16 +1196,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1387,7 +1387,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1401,7 +1401,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1928,25 +1928,25 @@
   <sheetPr/>
   <dimension ref="A1:AZ24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="66" topLeftCell="AK1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AK1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AS6" sqref="AS6"/>
+      <selection pane="bottomLeft" activeCell="AT24" sqref="AT24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.4296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" style="1" customWidth="1"/>
-    <col min="5" max="40" width="17.8359375" style="1" customWidth="1"/>
-    <col min="41" max="41" width="31.4296875" style="1" customWidth="1"/>
-    <col min="42" max="46" width="18.9453125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="18.9453125" style="16" customWidth="1"/>
-    <col min="48" max="51" width="18.9453125" style="1" customWidth="1"/>
-    <col min="52" max="52" width="18.9453125" style="16" customWidth="1"/>
-    <col min="53" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.42857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.552380952381" style="1" customWidth="1"/>
+    <col min="5" max="40" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="41" max="41" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="42" max="46" width="18.9428571428571" style="1" customWidth="1"/>
+    <col min="47" max="47" width="18.9428571428571" style="16" customWidth="1"/>
+    <col min="48" max="51" width="18.9428571428571" style="1" customWidth="1"/>
+    <col min="52" max="52" width="18.9428571428571" style="16" customWidth="1"/>
+    <col min="53" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="46" customHeight="1" spans="1:52">
@@ -2232,8 +2232,8 @@
       <c r="AT2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU2" s="16" t="s">
-        <v>63</v>
+      <c r="AU2" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV2" s="1" t="s">
         <v>78</v>
@@ -2247,8 +2247,8 @@
       <c r="AY2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ2" s="16" t="s">
-        <v>63</v>
+      <c r="AZ2" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="69" customHeight="1" spans="1:52">
@@ -2376,8 +2376,8 @@
       <c r="AT3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AU3" s="16" t="s">
-        <v>63</v>
+      <c r="AU3" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV3" s="1" t="s">
         <v>78</v>
@@ -2391,8 +2391,8 @@
       <c r="AY3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ3" s="16" t="s">
-        <v>63</v>
+      <c r="AZ3" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="69" customHeight="1" spans="1:52">
@@ -2524,8 +2524,8 @@
       <c r="AT4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU4" s="16" t="s">
-        <v>63</v>
+      <c r="AU4" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV4" s="1" t="s">
         <v>78</v>
@@ -2539,16 +2539,16 @@
       <c r="AY4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ4" s="16" t="s">
-        <v>91</v>
+      <c r="AZ4" s="16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="69" customHeight="1" spans="1:52">
       <c r="A5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>54</v>
@@ -2604,13 +2604,13 @@
         <v>56</v>
       </c>
       <c r="V5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="W5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="W5" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="X5" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Y5" s="7" t="s">
         <v>66</v>
@@ -2672,8 +2672,8 @@
       <c r="AT5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AU5" s="16" t="s">
-        <v>63</v>
+      <c r="AU5" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV5" s="1" t="s">
         <v>78</v>
@@ -2687,16 +2687,16 @@
       <c r="AY5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ5" s="16" t="s">
-        <v>91</v>
+      <c r="AZ5" s="16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="234" customHeight="1" spans="1:52">
       <c r="A6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>54</v>
@@ -2752,7 +2752,7 @@
         <v>56</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W6" s="7"/>
       <c r="X6" s="7"/>
@@ -2772,7 +2772,7 @@
         <v>90</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE6" s="7"/>
       <c r="AF6" s="7" t="s">
@@ -2794,7 +2794,7 @@
         <v>75</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
@@ -2816,8 +2816,8 @@
       <c r="AT6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU6" s="16" t="s">
-        <v>63</v>
+      <c r="AU6" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV6" s="1" t="s">
         <v>78</v>
@@ -2831,16 +2831,16 @@
       <c r="AY6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ6" s="16" t="s">
-        <v>63</v>
+      <c r="AZ6" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="69" customHeight="1" spans="1:52">
       <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>54</v>
@@ -2896,7 +2896,7 @@
         <v>56</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
@@ -2938,7 +2938,7 @@
         <v>75</v>
       </c>
       <c r="AL7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
@@ -2960,8 +2960,8 @@
       <c r="AT7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU7" s="16" t="s">
-        <v>63</v>
+      <c r="AU7" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV7" s="1" t="s">
         <v>78</v>
@@ -2975,16 +2975,16 @@
       <c r="AY7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ7" s="16" t="s">
-        <v>63</v>
+      <c r="AZ7" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="69" customHeight="1" spans="1:52">
       <c r="A8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>54</v>
@@ -3040,7 +3040,7 @@
         <v>56</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W8" s="7"/>
       <c r="X8" s="7"/>
@@ -3054,10 +3054,10 @@
         <v>68</v>
       </c>
       <c r="AB8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC8" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AC8" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AD8" s="7" t="s">
         <v>62</v>
@@ -3082,7 +3082,7 @@
         <v>75</v>
       </c>
       <c r="AL8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
@@ -3104,8 +3104,8 @@
       <c r="AT8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU8" s="16" t="s">
-        <v>63</v>
+      <c r="AU8" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV8" s="1" t="s">
         <v>78</v>
@@ -3119,16 +3119,16 @@
       <c r="AY8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ8" s="16" t="s">
-        <v>63</v>
+      <c r="AZ8" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" ht="69" customHeight="1" spans="1:52">
       <c r="A9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>54</v>
@@ -3184,7 +3184,7 @@
         <v>56</v>
       </c>
       <c r="V9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
@@ -3198,10 +3198,10 @@
         <v>68</v>
       </c>
       <c r="AB9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC9" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AD9" s="7" t="s">
         <v>66</v>
@@ -3226,7 +3226,7 @@
         <v>75</v>
       </c>
       <c r="AL9" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
@@ -3248,8 +3248,8 @@
       <c r="AT9" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU9" s="16" t="s">
-        <v>63</v>
+      <c r="AU9" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV9" s="1" t="s">
         <v>78</v>
@@ -3263,16 +3263,16 @@
       <c r="AY9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ9" s="16" t="s">
-        <v>63</v>
+      <c r="AZ9" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" ht="69" customHeight="1" spans="1:52">
       <c r="A10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>54</v>
@@ -3328,7 +3328,7 @@
         <v>56</v>
       </c>
       <c r="V10" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="W10" s="7"/>
       <c r="X10" s="7"/>
@@ -3342,13 +3342,13 @@
         <v>68</v>
       </c>
       <c r="AB10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AC10" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="AD10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE10" s="7"/>
       <c r="AF10" s="7" t="s">
@@ -3370,7 +3370,7 @@
         <v>75</v>
       </c>
       <c r="AL10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AM10" s="7"/>
       <c r="AN10" s="7"/>
@@ -3392,8 +3392,8 @@
       <c r="AT10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU10" s="16" t="s">
-        <v>63</v>
+      <c r="AU10" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV10" s="1" t="s">
         <v>78</v>
@@ -3407,16 +3407,16 @@
       <c r="AY10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ10" s="16" t="s">
-        <v>63</v>
+      <c r="AZ10" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" ht="69" customHeight="1" spans="1:52">
       <c r="A11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>54</v>
@@ -3472,7 +3472,7 @@
         <v>56</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
@@ -3486,10 +3486,10 @@
         <v>68</v>
       </c>
       <c r="AB11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC11" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AC11" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>83</v>
@@ -3514,7 +3514,7 @@
         <v>75</v>
       </c>
       <c r="AL11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
@@ -3536,8 +3536,8 @@
       <c r="AT11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU11" s="16" t="s">
-        <v>63</v>
+      <c r="AU11" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV11" s="1" t="s">
         <v>78</v>
@@ -3551,16 +3551,16 @@
       <c r="AY11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ11" s="16" t="s">
-        <v>63</v>
+      <c r="AZ11" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" ht="69" customHeight="1" spans="1:52">
       <c r="A12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>54</v>
@@ -3616,7 +3616,7 @@
         <v>56</v>
       </c>
       <c r="V12" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
@@ -3630,10 +3630,10 @@
         <v>68</v>
       </c>
       <c r="AB12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC12" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AC12" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AD12" s="7" t="s">
         <v>62</v>
@@ -3658,7 +3658,7 @@
         <v>75</v>
       </c>
       <c r="AL12" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
@@ -3680,8 +3680,8 @@
       <c r="AT12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU12" s="16" t="s">
-        <v>63</v>
+      <c r="AU12" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV12" s="1" t="s">
         <v>78</v>
@@ -3695,16 +3695,16 @@
       <c r="AY12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ12" s="16" t="s">
-        <v>63</v>
+      <c r="AZ12" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" ht="69" customHeight="1" spans="1:52">
       <c r="A13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>54</v>
@@ -3760,7 +3760,7 @@
         <v>56</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
@@ -3774,10 +3774,10 @@
         <v>68</v>
       </c>
       <c r="AB13" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC13" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AC13" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AD13" s="7" t="s">
         <v>66</v>
@@ -3802,7 +3802,7 @@
         <v>75</v>
       </c>
       <c r="AL13" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
@@ -3824,8 +3824,8 @@
       <c r="AT13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU13" s="16" t="s">
-        <v>63</v>
+      <c r="AU13" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV13" s="1" t="s">
         <v>78</v>
@@ -3839,16 +3839,16 @@
       <c r="AY13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ13" s="16" t="s">
-        <v>63</v>
+      <c r="AZ13" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" ht="69" customHeight="1" spans="1:52">
       <c r="A14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>54</v>
@@ -3904,7 +3904,7 @@
         <v>56</v>
       </c>
       <c r="V14" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
@@ -3918,13 +3918,13 @@
         <v>68</v>
       </c>
       <c r="AB14" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC14" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AC14" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="AD14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7" t="s">
@@ -3946,7 +3946,7 @@
         <v>75</v>
       </c>
       <c r="AL14" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
@@ -3968,8 +3968,8 @@
       <c r="AT14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU14" s="16" t="s">
-        <v>63</v>
+      <c r="AU14" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV14" s="1" t="s">
         <v>78</v>
@@ -3983,16 +3983,16 @@
       <c r="AY14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ14" s="16" t="s">
-        <v>63</v>
+      <c r="AZ14" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" ht="69" customHeight="1" spans="1:52">
       <c r="A15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>54</v>
@@ -4048,7 +4048,7 @@
         <v>56</v>
       </c>
       <c r="V15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
@@ -4062,10 +4062,10 @@
         <v>68</v>
       </c>
       <c r="AB15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC15" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AC15" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AD15" s="7" t="s">
         <v>83</v>
@@ -4090,7 +4090,7 @@
         <v>75</v>
       </c>
       <c r="AL15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AM15" s="7"/>
       <c r="AN15" s="7"/>
@@ -4112,8 +4112,8 @@
       <c r="AT15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU15" s="16" t="s">
-        <v>63</v>
+      <c r="AU15" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV15" s="1" t="s">
         <v>78</v>
@@ -4127,16 +4127,16 @@
       <c r="AY15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ15" s="16" t="s">
-        <v>63</v>
+      <c r="AZ15" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" ht="69" customHeight="1" spans="1:52">
       <c r="A16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>54</v>
@@ -4192,7 +4192,7 @@
         <v>56</v>
       </c>
       <c r="V16" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
@@ -4206,10 +4206,10 @@
         <v>68</v>
       </c>
       <c r="AB16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC16" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AC16" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AD16" s="7" t="s">
         <v>62</v>
@@ -4234,7 +4234,7 @@
         <v>75</v>
       </c>
       <c r="AL16" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AM16" s="7"/>
       <c r="AN16" s="7"/>
@@ -4256,8 +4256,8 @@
       <c r="AT16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU16" s="16" t="s">
-        <v>63</v>
+      <c r="AU16" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV16" s="1" t="s">
         <v>78</v>
@@ -4271,16 +4271,16 @@
       <c r="AY16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ16" s="16" t="s">
-        <v>63</v>
+      <c r="AZ16" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" ht="69" customHeight="1" spans="1:52">
       <c r="A17" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>54</v>
@@ -4336,7 +4336,7 @@
         <v>56</v>
       </c>
       <c r="V17" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
@@ -4350,10 +4350,10 @@
         <v>68</v>
       </c>
       <c r="AB17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC17" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AC17" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AD17" s="7" t="s">
         <v>66</v>
@@ -4378,7 +4378,7 @@
         <v>75</v>
       </c>
       <c r="AL17" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AM17" s="7"/>
       <c r="AN17" s="7"/>
@@ -4400,8 +4400,8 @@
       <c r="AT17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU17" s="16" t="s">
-        <v>63</v>
+      <c r="AU17" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV17" s="1" t="s">
         <v>78</v>
@@ -4415,16 +4415,16 @@
       <c r="AY17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ17" s="16" t="s">
-        <v>63</v>
+      <c r="AZ17" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" ht="69" customHeight="1" spans="1:52">
       <c r="A18" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>54</v>
@@ -4480,7 +4480,7 @@
         <v>56</v>
       </c>
       <c r="V18" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
@@ -4494,13 +4494,13 @@
         <v>68</v>
       </c>
       <c r="AB18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC18" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AC18" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="AD18" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AE18" s="7"/>
       <c r="AF18" s="7" t="s">
@@ -4522,7 +4522,7 @@
         <v>75</v>
       </c>
       <c r="AL18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
@@ -4544,8 +4544,8 @@
       <c r="AT18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU18" s="16" t="s">
-        <v>63</v>
+      <c r="AU18" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV18" s="1" t="s">
         <v>78</v>
@@ -4559,16 +4559,16 @@
       <c r="AY18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ18" s="16" t="s">
-        <v>63</v>
+      <c r="AZ18" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" ht="69" customHeight="1" spans="1:52">
       <c r="A19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>54</v>
@@ -4624,7 +4624,7 @@
         <v>56</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
@@ -4638,10 +4638,10 @@
         <v>68</v>
       </c>
       <c r="AB19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC19" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AC19" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AD19" s="7" t="s">
         <v>83</v>
@@ -4666,7 +4666,7 @@
         <v>75</v>
       </c>
       <c r="AL19" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AM19" s="7"/>
       <c r="AN19" s="7"/>
@@ -4688,8 +4688,8 @@
       <c r="AT19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU19" s="16" t="s">
-        <v>63</v>
+      <c r="AU19" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV19" s="1" t="s">
         <v>78</v>
@@ -4703,16 +4703,16 @@
       <c r="AY19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ19" s="16" t="s">
-        <v>63</v>
+      <c r="AZ19" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" ht="69" customHeight="1" spans="1:52">
       <c r="A20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>159</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>160</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>54</v>
@@ -4768,7 +4768,7 @@
         <v>56</v>
       </c>
       <c r="V20" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
@@ -4782,10 +4782,10 @@
         <v>68</v>
       </c>
       <c r="AB20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC20" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="AC20" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="AD20" s="7" t="s">
         <v>62</v>
@@ -4810,7 +4810,7 @@
         <v>75</v>
       </c>
       <c r="AL20" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AM20" s="7"/>
       <c r="AN20" s="7"/>
@@ -4832,8 +4832,8 @@
       <c r="AT20" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU20" s="16" t="s">
-        <v>63</v>
+      <c r="AU20" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV20" s="1" t="s">
         <v>78</v>
@@ -4847,16 +4847,16 @@
       <c r="AY20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ20" s="16" t="s">
-        <v>63</v>
+      <c r="AZ20" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" ht="69" customHeight="1" spans="1:52">
       <c r="A21" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>166</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>54</v>
@@ -4912,7 +4912,7 @@
         <v>56</v>
       </c>
       <c r="V21" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
@@ -4926,10 +4926,10 @@
         <v>68</v>
       </c>
       <c r="AB21" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC21" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="AC21" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="AD21" s="7" t="s">
         <v>66</v>
@@ -4954,7 +4954,7 @@
         <v>75</v>
       </c>
       <c r="AL21" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AM21" s="7"/>
       <c r="AN21" s="7"/>
@@ -4976,8 +4976,8 @@
       <c r="AT21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AU21" s="16" t="s">
-        <v>63</v>
+      <c r="AU21" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="AV21" s="1" t="s">
         <v>78</v>
@@ -4991,19 +4991,19 @@
       <c r="AY21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AZ21" s="16" t="s">
-        <v>63</v>
+      <c r="AZ21" s="16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" ht="69" customHeight="1" spans="1:42">
       <c r="A22" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>55</v>
@@ -5099,7 +5099,7 @@
       <c r="AM22" s="7"/>
       <c r="AN22" s="7"/>
       <c r="AO22" s="13" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="AP22" s="1">
         <v>500</v>
@@ -5113,7 +5113,7 @@
         <v>173</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>55</v>
@@ -5211,7 +5211,7 @@
       <c r="AM23" s="7"/>
       <c r="AN23" s="7"/>
       <c r="AO23" s="13" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="AP23" s="1">
         <v>500</v>
@@ -5225,7 +5225,7 @@
         <v>177</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>55</v>
@@ -5323,7 +5323,7 @@
       <c r="AM24" s="7"/>
       <c r="AN24" s="7"/>
       <c r="AO24" s="13" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
       <c r="AP24" s="1">
         <v>500</v>
@@ -5344,16 +5344,16 @@
       <selection activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.4296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
-    <col min="4" max="39" width="17.8359375" style="1" customWidth="1"/>
-    <col min="40" max="40" width="31.4296875" style="1" customWidth="1"/>
-    <col min="41" max="41" width="32.2890625" style="1" customWidth="1"/>
-    <col min="42" max="44" width="21.9921875" style="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8.42857142857143" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7142857142857" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="39" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="40" max="40" width="31.4285714285714" style="1" customWidth="1"/>
+    <col min="41" max="41" width="32.2857142857143" style="1" customWidth="1"/>
+    <col min="42" max="44" width="21.9904761904762" style="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="46" customHeight="1" spans="1:44">
@@ -5856,10 +5856,10 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>54</v>
@@ -5912,13 +5912,13 @@
         <v>56</v>
       </c>
       <c r="U5" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="V5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="V5" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="W5" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="X5" s="7" t="s">
         <v>66</v>
@@ -5980,10 +5980,10 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>96</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>97</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>54</v>
@@ -6036,7 +6036,7 @@
         <v>56</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V6" s="7"/>
       <c r="W6" s="7"/>
@@ -6056,7 +6056,7 @@
         <v>90</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD6" s="7"/>
       <c r="AE6" s="7" t="s">
@@ -6078,7 +6078,7 @@
         <v>75</v>
       </c>
       <c r="AK6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
@@ -6100,10 +6100,10 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>54</v>
@@ -6156,7 +6156,7 @@
         <v>56</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="V7" s="7"/>
       <c r="W7" s="7"/>
@@ -6198,7 +6198,7 @@
         <v>75</v>
       </c>
       <c r="AK7" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
@@ -6220,10 +6220,10 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A8" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>54</v>
@@ -6276,7 +6276,7 @@
         <v>56</v>
       </c>
       <c r="U8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V8" s="7"/>
       <c r="W8" s="7"/>
@@ -6290,10 +6290,10 @@
         <v>68</v>
       </c>
       <c r="AA8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB8" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AB8" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>62</v>
@@ -6318,7 +6318,7 @@
         <v>75</v>
       </c>
       <c r="AK8" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
@@ -6340,10 +6340,10 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>54</v>
@@ -6396,7 +6396,7 @@
         <v>56</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
@@ -6410,10 +6410,10 @@
         <v>68</v>
       </c>
       <c r="AA9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB9" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AB9" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AC9" s="7" t="s">
         <v>66</v>
@@ -6438,7 +6438,7 @@
         <v>75</v>
       </c>
       <c r="AK9" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AL9" s="7"/>
       <c r="AM9" s="7"/>
@@ -6460,10 +6460,10 @@
     </row>
     <row r="10" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>54</v>
@@ -6516,7 +6516,7 @@
         <v>56</v>
       </c>
       <c r="U10" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
@@ -6530,13 +6530,13 @@
         <v>68</v>
       </c>
       <c r="AA10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB10" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AB10" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="AC10" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD10" s="7"/>
       <c r="AE10" s="7" t="s">
@@ -6558,7 +6558,7 @@
         <v>75</v>
       </c>
       <c r="AK10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AL10" s="7"/>
       <c r="AM10" s="7"/>
@@ -6580,10 +6580,10 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A11" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>119</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>54</v>
@@ -6636,7 +6636,7 @@
         <v>56</v>
       </c>
       <c r="U11" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
@@ -6650,10 +6650,10 @@
         <v>68</v>
       </c>
       <c r="AA11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB11" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="AB11" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="AC11" s="7" t="s">
         <v>83</v>
@@ -6678,7 +6678,7 @@
         <v>75</v>
       </c>
       <c r="AK11" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AL11" s="7"/>
       <c r="AM11" s="7"/>
@@ -6700,10 +6700,10 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>54</v>
@@ -6756,7 +6756,7 @@
         <v>56</v>
       </c>
       <c r="U12" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
@@ -6770,10 +6770,10 @@
         <v>68</v>
       </c>
       <c r="AA12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB12" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AB12" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AC12" s="7" t="s">
         <v>62</v>
@@ -6798,7 +6798,7 @@
         <v>75</v>
       </c>
       <c r="AK12" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL12" s="7"/>
       <c r="AM12" s="7"/>
@@ -6820,10 +6820,10 @@
     </row>
     <row r="13" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A13" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>54</v>
@@ -6876,7 +6876,7 @@
         <v>56</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
@@ -6890,10 +6890,10 @@
         <v>68</v>
       </c>
       <c r="AA13" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB13" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AB13" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AC13" s="7" t="s">
         <v>66</v>
@@ -6918,7 +6918,7 @@
         <v>75</v>
       </c>
       <c r="AK13" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL13" s="7"/>
       <c r="AM13" s="7"/>
@@ -6940,10 +6940,10 @@
     </row>
     <row r="14" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A14" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>54</v>
@@ -6996,7 +6996,7 @@
         <v>56</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V14" s="7"/>
       <c r="W14" s="7"/>
@@ -7010,13 +7010,13 @@
         <v>68</v>
       </c>
       <c r="AA14" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB14" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AB14" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="AC14" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD14" s="7"/>
       <c r="AE14" s="7" t="s">
@@ -7038,7 +7038,7 @@
         <v>75</v>
       </c>
       <c r="AK14" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="AL14" s="7"/>
       <c r="AM14" s="7"/>
@@ -7060,10 +7060,10 @@
     </row>
     <row r="15" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A15" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>138</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>54</v>
@@ -7116,7 +7116,7 @@
         <v>56</v>
       </c>
       <c r="U15" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V15" s="7"/>
       <c r="W15" s="7"/>
@@ -7130,10 +7130,10 @@
         <v>68</v>
       </c>
       <c r="AA15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB15" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="AB15" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="AC15" s="7" t="s">
         <v>83</v>
@@ -7158,7 +7158,7 @@
         <v>75</v>
       </c>
       <c r="AK15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AL15" s="7"/>
       <c r="AM15" s="7"/>
@@ -7180,10 +7180,10 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A16" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>141</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>54</v>
@@ -7236,7 +7236,7 @@
         <v>56</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
@@ -7250,10 +7250,10 @@
         <v>68</v>
       </c>
       <c r="AA16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB16" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AB16" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AC16" s="7" t="s">
         <v>62</v>
@@ -7278,7 +7278,7 @@
         <v>75</v>
       </c>
       <c r="AK16" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AL16" s="7"/>
       <c r="AM16" s="7"/>
@@ -7300,10 +7300,10 @@
     </row>
     <row r="17" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A17" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>54</v>
@@ -7356,7 +7356,7 @@
         <v>56</v>
       </c>
       <c r="U17" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
@@ -7370,10 +7370,10 @@
         <v>68</v>
       </c>
       <c r="AA17" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB17" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AB17" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AC17" s="7" t="s">
         <v>66</v>
@@ -7398,7 +7398,7 @@
         <v>75</v>
       </c>
       <c r="AK17" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AL17" s="7"/>
       <c r="AM17" s="7"/>
@@ -7420,10 +7420,10 @@
     </row>
     <row r="18" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A18" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>152</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>54</v>
@@ -7476,7 +7476,7 @@
         <v>56</v>
       </c>
       <c r="U18" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
@@ -7490,13 +7490,13 @@
         <v>68</v>
       </c>
       <c r="AA18" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB18" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AB18" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="AC18" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AD18" s="7"/>
       <c r="AE18" s="7" t="s">
@@ -7518,7 +7518,7 @@
         <v>75</v>
       </c>
       <c r="AK18" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AL18" s="7"/>
       <c r="AM18" s="7"/>
@@ -7540,10 +7540,10 @@
     </row>
     <row r="19" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A19" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>54</v>
@@ -7596,7 +7596,7 @@
         <v>56</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
@@ -7610,10 +7610,10 @@
         <v>68</v>
       </c>
       <c r="AA19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB19" s="7" t="s">
         <v>144</v>
-      </c>
-      <c r="AB19" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="AC19" s="7" t="s">
         <v>83</v>
@@ -7638,7 +7638,7 @@
         <v>75</v>
       </c>
       <c r="AK19" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AL19" s="7"/>
       <c r="AM19" s="7"/>
@@ -7660,10 +7660,10 @@
     </row>
     <row r="20" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>159</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>160</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>54</v>
@@ -7716,7 +7716,7 @@
         <v>56</v>
       </c>
       <c r="U20" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
@@ -7730,10 +7730,10 @@
         <v>68</v>
       </c>
       <c r="AA20" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB20" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="AB20" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="AC20" s="7" t="s">
         <v>62</v>
@@ -7758,7 +7758,7 @@
         <v>75</v>
       </c>
       <c r="AK20" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AL20" s="7"/>
       <c r="AM20" s="7"/>
@@ -7780,10 +7780,10 @@
     </row>
     <row r="21" s="1" customFormat="1" ht="69" customHeight="1" spans="1:44">
       <c r="A21" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>166</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>54</v>
@@ -7836,7 +7836,7 @@
         <v>56</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
@@ -7850,10 +7850,10 @@
         <v>68</v>
       </c>
       <c r="AA21" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB21" s="7" t="s">
         <v>162</v>
-      </c>
-      <c r="AB21" s="7" t="s">
-        <v>163</v>
       </c>
       <c r="AC21" s="7" t="s">
         <v>66</v>
@@ -7878,7 +7878,7 @@
         <v>75</v>
       </c>
       <c r="AK21" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AL21" s="7"/>
       <c r="AM21" s="7"/>
@@ -7900,13 +7900,13 @@
     </row>
     <row r="22" s="1" customFormat="1" ht="69" customHeight="1" spans="1:41">
       <c r="A22" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>56</v>
@@ -8011,7 +8011,7 @@
         <v>173</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>56</v>
@@ -8118,7 +8118,7 @@
         <v>177</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
update create booking tc
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="13100" activeTab="3"/>
+    <workbookView windowWidth="30240" windowHeight="13100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="230">
   <si>
     <t>tc_id</t>
   </si>
@@ -650,6 +650,9 @@
   </si>
   <si>
     <t>AG_Kiểm tra booking 1 player có đặt caddie</t>
+  </si>
+  <si>
+    <t>NG_Kiểm tra booking none golf</t>
   </si>
   <si>
     <t>EB_VST_001</t>
@@ -8411,8 +8414,8 @@
   <sheetPr/>
   <dimension ref="A1:AZ24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
@@ -8940,7 +8943,9 @@
       <c r="A8" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
       <c r="E8" s="5"/>
@@ -9899,8 +9904,8 @@
   <sheetPr/>
   <dimension ref="A1:AZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1"/>
@@ -10078,10 +10083,10 @@
     </row>
     <row r="2" s="1" customFormat="1" ht="50" customHeight="1" spans="1:52">
       <c r="A2" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -10136,10 +10141,10 @@
     </row>
     <row r="3" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A3" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="7"/>
@@ -10194,10 +10199,10 @@
     </row>
     <row r="4" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A4" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="7"/>
@@ -10252,10 +10257,10 @@
     </row>
     <row r="5" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A5" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="7"/>
@@ -10310,10 +10315,10 @@
     </row>
     <row r="6" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A6" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="7"/>
@@ -10368,10 +10373,10 @@
     </row>
     <row r="7" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A7" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
@@ -10426,10 +10431,10 @@
     </row>
     <row r="8" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A8" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7"/>
@@ -10484,10 +10489,10 @@
     </row>
     <row r="9" s="1" customFormat="1" ht="80" customHeight="1" spans="1:52">
       <c r="A9" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="7"/>
@@ -10542,10 +10547,10 @@
     </row>
     <row r="10" s="1" customFormat="1" ht="68" customHeight="1" spans="1:52">
       <c r="A10" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7"/>
@@ -10600,10 +10605,10 @@
     </row>
     <row r="11" s="1" customFormat="1" ht="86" customHeight="1" spans="1:52">
       <c r="A11" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7"/>
@@ -10658,10 +10663,10 @@
     </row>
     <row r="12" s="1" customFormat="1" ht="67" customHeight="1" spans="1:52">
       <c r="A12" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
@@ -10716,10 +10721,10 @@
     </row>
     <row r="13" s="1" customFormat="1" ht="58" customHeight="1" spans="1:52">
       <c r="A13" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
@@ -10774,7 +10779,7 @@
     </row>
     <row r="14" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A14" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="8"/>
@@ -10830,7 +10835,7 @@
     </row>
     <row r="15" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A15" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="8"/>
@@ -10886,7 +10891,7 @@
     </row>
     <row r="16" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A16" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>
@@ -10942,7 +10947,7 @@
     </row>
     <row r="17" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A17" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="8"/>
@@ -10998,7 +11003,7 @@
     </row>
     <row r="18" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A18" s="4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="8"/>
@@ -11054,7 +11059,7 @@
     </row>
     <row r="19" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A19" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="8"/>
@@ -11110,7 +11115,7 @@
     </row>
     <row r="20" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A20" s="4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="8"/>
@@ -11166,7 +11171,7 @@
     </row>
     <row r="21" s="1" customFormat="1" ht="69" customHeight="1" spans="1:52">
       <c r="A21" s="4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="8"/>

</xml_diff>

<commit_message>
update report show log flow
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
+++ b/src/main/resources/input_excel_file/booking/Create_Booking_Batch.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11460"/>
+    <workbookView windowWidth="28800" windowHeight="11460" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="quote_fee_1_player" sheetId="6" r:id="rId1"/>
@@ -2823,7 +2823,7 @@
       <charset val="0"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2863,12 +2863,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3287,7 +3281,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3311,16 +3305,16 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -3329,89 +3323,89 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3622,28 +3616,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4228,16 +4204,16 @@
   <sheetPr/>
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="$A6:$XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.5333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6857142857143" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.552380952381" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.4285714285714" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.2857142857143" style="1" customWidth="1"/>
     <col min="5" max="24" width="17.8380952380952" style="1" customWidth="1"/>
     <col min="25" max="25" width="31.4285714285714" style="1" customWidth="1"/>
     <col min="26" max="30" width="18.9428571428571" style="1" customWidth="1"/>
@@ -4357,14 +4333,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A2" s="4" t="s">
+    <row r="2" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -4386,7 +4362,7 @@
       <c r="J2" s="7">
         <v>1</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="69" t="s">
         <v>44</v>
       </c>
       <c r="L2" s="7">
@@ -4395,162 +4371,162 @@
       <c r="M2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="69">
         <v>100</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
       <c r="Y2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="9">
+      <c r="Z2" s="26">
         <v>200</v>
       </c>
-      <c r="AA2" s="9">
+      <c r="AA2" s="26">
         <v>1</v>
       </c>
-      <c r="AB2" s="9">
+      <c r="AB2" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC2" s="9">
+      <c r="AC2" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD2" s="9">
+      <c r="AD2" s="26">
         <f>AE2+AF2</f>
         <v>1600000</v>
       </c>
-      <c r="AE2" s="19">
+      <c r="AE2" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF2" s="9">
+      <c r="AF2" s="26">
         <v>600000</v>
       </c>
-      <c r="AG2" s="9">
+      <c r="AG2" s="26">
         <v>400000</v>
       </c>
-      <c r="AH2" s="9">
+      <c r="AH2" s="26">
         <f t="shared" ref="AH2:AH10" si="0">L2</f>
         <v>18</v>
       </c>
-      <c r="AI2" s="9" t="str">
+      <c r="AI2" s="26" t="str">
         <f t="shared" ref="AI2:AI10" si="1">H2</f>
         <v>4D</v>
       </c>
-      <c r="AJ2" s="19">
+      <c r="AJ2" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="3" s="66" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A3" s="4" t="s">
+    <row r="3" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H3" s="56">
+      <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56">
+      <c r="I3" s="7"/>
+      <c r="J3" s="7">
         <v>1</v>
       </c>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="56">
+      <c r="L3" s="7">
         <v>18</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="56">
+      <c r="N3" s="7">
         <v>102</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z3" s="58">
+      <c r="Z3" s="26">
         <v>200</v>
       </c>
-      <c r="AA3" s="58">
+      <c r="AA3" s="26">
         <v>1</v>
       </c>
-      <c r="AB3" s="58">
+      <c r="AB3" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC3" s="58">
+      <c r="AC3" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD3" s="58">
+      <c r="AD3" s="26">
         <f>AE3+AF3</f>
         <v>1600000</v>
       </c>
-      <c r="AE3" s="74">
+      <c r="AE3" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF3" s="58">
+      <c r="AF3" s="26">
         <v>600000</v>
       </c>
-      <c r="AG3" s="58">
+      <c r="AG3" s="26">
         <v>400000</v>
       </c>
-      <c r="AH3" s="58">
+      <c r="AH3" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI3" s="58">
+      <c r="AI3" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AJ3" s="74">
+      <c r="AJ3" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A4" s="4" t="s">
+    <row r="4" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A4" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -4568,11 +4544,11 @@
       <c r="H4" s="7">
         <v>2</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="69" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="7">
@@ -4587,63 +4563,63 @@
       <c r="O4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
-      <c r="R4" s="73"/>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="26"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="9">
+      <c r="Z4" s="26">
         <v>200</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="26">
         <v>1</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AB4" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AC4" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD4" s="9">
+      <c r="AD4" s="26">
         <f>AE4+AF4</f>
         <v>1600000</v>
       </c>
-      <c r="AE4" s="19">
+      <c r="AE4" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF4" s="26">
         <v>600000</v>
       </c>
-      <c r="AG4" s="9">
+      <c r="AG4" s="26">
         <v>400000</v>
       </c>
-      <c r="AH4" s="9">
+      <c r="AH4" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AI4" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AJ4" s="19">
+      <c r="AJ4" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="5" s="66" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A5" s="4" t="s">
+    <row r="5" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -4661,11 +4637,11 @@
       <c r="H5" s="7">
         <v>7</v>
       </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="26"/>
       <c r="J5" s="7">
         <v>1</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="69" t="s">
         <v>54</v>
       </c>
       <c r="L5" s="7">
@@ -4680,155 +4656,155 @@
       <c r="O5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="73"/>
-      <c r="V5" s="73"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
       <c r="Y5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z5" s="9">
+      <c r="Z5" s="26">
         <v>200</v>
       </c>
-      <c r="AA5" s="9">
+      <c r="AA5" s="26">
         <v>1</v>
       </c>
-      <c r="AB5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="19">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="9">
+      <c r="AB5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="65">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="26">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI5" s="9">
+      <c r="AI5" s="26">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AJ5" s="19">
+      <c r="AJ5" s="65">
         <v>23456710</v>
       </c>
     </row>
-    <row r="6" s="66" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A6" s="4" t="s">
+    <row r="6" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="56">
+      <c r="I6" s="26"/>
+      <c r="J6" s="7">
         <v>1</v>
       </c>
-      <c r="K6" s="72" t="s">
+      <c r="K6" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="56">
+      <c r="L6" s="7">
         <v>18</v>
       </c>
-      <c r="M6" s="56" t="s">
+      <c r="M6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="56">
+      <c r="N6" s="7">
         <v>106</v>
       </c>
-      <c r="O6" s="56" t="s">
+      <c r="O6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="56" t="s">
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z6" s="58">
+      <c r="Z6" s="26">
         <v>200</v>
       </c>
-      <c r="AA6" s="58">
+      <c r="AA6" s="26">
         <v>1</v>
       </c>
-      <c r="AB6" s="58">
+      <c r="AB6" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC6" s="58">
+      <c r="AC6" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD6" s="58">
+      <c r="AD6" s="26">
         <f>AE6+AF6</f>
         <v>1600000</v>
       </c>
-      <c r="AE6" s="74">
+      <c r="AE6" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF6" s="58">
+      <c r="AF6" s="26">
         <v>600000</v>
       </c>
-      <c r="AG6" s="58">
+      <c r="AG6" s="26">
         <v>400000</v>
       </c>
-      <c r="AH6" s="58">
+      <c r="AH6" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI6" s="58" t="str">
+      <c r="AI6" s="26" t="str">
         <f t="shared" si="1"/>
         <v>5D</v>
       </c>
-      <c r="AJ6" s="74">
+      <c r="AJ6" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A7" s="4" t="s">
+    <row r="7" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A7" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -4846,13 +4822,13 @@
       <c r="H7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="75" t="s">
+      <c r="I7" s="70" t="s">
         <v>60</v>
       </c>
       <c r="J7" s="7">
         <v>1</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="69" t="s">
         <v>44</v>
       </c>
       <c r="L7" s="7">
@@ -4867,158 +4843,158 @@
       <c r="O7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
-      <c r="T7" s="71"/>
-      <c r="U7" s="71"/>
-      <c r="V7" s="71"/>
-      <c r="W7" s="71"/>
-      <c r="X7" s="71"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
       <c r="Y7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z7" s="9">
+      <c r="Z7" s="26">
         <v>200</v>
       </c>
-      <c r="AA7" s="9">
+      <c r="AA7" s="26">
         <v>1</v>
       </c>
-      <c r="AB7" s="9">
+      <c r="AB7" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC7" s="9">
+      <c r="AC7" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD7" s="9">
+      <c r="AD7" s="26">
         <f>AE7+AF7</f>
         <v>1600000</v>
       </c>
-      <c r="AE7" s="19">
+      <c r="AE7" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF7" s="9">
+      <c r="AF7" s="26">
         <v>600000</v>
       </c>
-      <c r="AG7" s="9">
+      <c r="AG7" s="26">
         <v>400000</v>
       </c>
-      <c r="AH7" s="9">
+      <c r="AH7" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI7" s="9" t="str">
+      <c r="AI7" s="26" t="str">
         <f t="shared" si="1"/>
         <v>4D</v>
       </c>
-      <c r="AJ7" s="19">
+      <c r="AJ7" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="8" s="66" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A8" s="4" t="s">
+    <row r="8" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A8" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="56" t="s">
+      <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="56">
+      <c r="H8" s="7">
         <v>1</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="56">
+      <c r="J8" s="7">
         <v>1</v>
       </c>
-      <c r="K8" s="72" t="s">
+      <c r="K8" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="56">
+      <c r="L8" s="7">
         <v>18</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="M8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="56">
+      <c r="N8" s="7">
         <v>103</v>
       </c>
-      <c r="O8" s="56" t="s">
+      <c r="O8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="56" t="s">
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="26"/>
+      <c r="U8" s="26"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="26"/>
+      <c r="X8" s="26"/>
+      <c r="Y8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z8" s="58">
+      <c r="Z8" s="26">
         <v>200</v>
       </c>
-      <c r="AA8" s="58">
+      <c r="AA8" s="26">
         <v>1</v>
       </c>
-      <c r="AB8" s="58">
+      <c r="AB8" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC8" s="58">
+      <c r="AC8" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD8" s="58">
+      <c r="AD8" s="26">
         <f>AE8+AF8</f>
         <v>1600000</v>
       </c>
-      <c r="AE8" s="74">
+      <c r="AE8" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF8" s="58">
+      <c r="AF8" s="26">
         <v>600000</v>
       </c>
-      <c r="AG8" s="58">
+      <c r="AG8" s="26">
         <v>400000</v>
       </c>
-      <c r="AH8" s="58">
+      <c r="AH8" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI8" s="58">
+      <c r="AI8" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AJ8" s="74">
+      <c r="AJ8" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="9" ht="43" customHeight="1" spans="1:36">
-      <c r="A9" s="4" t="s">
+    <row r="9" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A9" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="57" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -5036,13 +5012,13 @@
       <c r="H9" s="7">
         <v>2</v>
       </c>
-      <c r="I9" s="77" t="s">
+      <c r="I9" s="71" t="s">
         <v>66</v>
       </c>
       <c r="J9" s="7">
         <v>1</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="69" t="s">
         <v>51</v>
       </c>
       <c r="L9" s="7">
@@ -5057,147 +5033,147 @@
       <c r="O9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="73"/>
-      <c r="R9" s="73"/>
-      <c r="S9" s="73"/>
-      <c r="T9" s="73"/>
-      <c r="U9" s="73"/>
-      <c r="V9" s="73"/>
-      <c r="W9" s="73"/>
-      <c r="X9" s="73"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="26"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="26"/>
+      <c r="X9" s="26"/>
       <c r="Y9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z9" s="9">
+      <c r="Z9" s="26">
         <v>200</v>
       </c>
-      <c r="AA9" s="9">
+      <c r="AA9" s="26">
         <v>1</v>
       </c>
-      <c r="AB9" s="9">
+      <c r="AB9" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC9" s="9">
+      <c r="AC9" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD9" s="9">
+      <c r="AD9" s="26">
         <f>AE9+AF9</f>
         <v>1600000</v>
       </c>
-      <c r="AE9" s="19">
+      <c r="AE9" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF9" s="9">
+      <c r="AF9" s="26">
         <v>600000</v>
       </c>
-      <c r="AG9" s="9">
+      <c r="AG9" s="26">
         <v>400000</v>
       </c>
-      <c r="AH9" s="9">
+      <c r="AH9" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI9" s="9">
+      <c r="AI9" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AJ9" s="19">
+      <c r="AJ9" s="65">
         <v>23456</v>
       </c>
     </row>
-    <row r="10" s="66" customFormat="1" ht="43" customHeight="1" spans="1:36">
-      <c r="A10" s="4" t="s">
+    <row r="10" s="54" customFormat="1" ht="43" customHeight="1" spans="1:36">
+      <c r="A10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="70" t="s">
+      <c r="C10" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="56" t="s">
+      <c r="F10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="56" t="s">
+      <c r="H10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="76" t="s">
+      <c r="I10" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="7">
         <v>1</v>
       </c>
-      <c r="K10" s="72" t="s">
+      <c r="K10" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="56">
+      <c r="L10" s="7">
         <v>18</v>
       </c>
-      <c r="M10" s="56" t="s">
+      <c r="M10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="56">
+      <c r="N10" s="7">
         <v>107</v>
       </c>
-      <c r="O10" s="56" t="s">
+      <c r="O10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="P10" s="58"/>
-      <c r="Q10" s="58"/>
-      <c r="R10" s="58"/>
-      <c r="S10" s="58"/>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="V10" s="58"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="58"/>
-      <c r="Y10" s="56" t="s">
+      <c r="P10" s="26"/>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="26"/>
+      <c r="S10" s="26"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+      <c r="X10" s="26"/>
+      <c r="Y10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="Z10" s="58">
+      <c r="Z10" s="26">
         <v>200</v>
       </c>
-      <c r="AA10" s="58">
+      <c r="AA10" s="26">
         <v>1</v>
       </c>
-      <c r="AB10" s="58">
+      <c r="AB10" s="26">
         <v>2000000</v>
       </c>
-      <c r="AC10" s="58">
+      <c r="AC10" s="26">
         <v>2000000</v>
       </c>
-      <c r="AD10" s="58">
+      <c r="AD10" s="26">
         <f>AE10+AF10</f>
         <v>1600000</v>
       </c>
-      <c r="AE10" s="74">
+      <c r="AE10" s="65">
         <v>1000000</v>
       </c>
-      <c r="AF10" s="58">
+      <c r="AF10" s="26">
         <v>600000</v>
       </c>
-      <c r="AG10" s="58">
+      <c r="AG10" s="26">
         <v>400000</v>
       </c>
-      <c r="AH10" s="58">
+      <c r="AH10" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AI10" s="58" t="str">
+      <c r="AI10" s="26" t="str">
         <f t="shared" si="1"/>
         <v>5D</v>
       </c>
-      <c r="AJ10" s="74">
+      <c r="AJ10" s="65">
         <v>23456</v>
       </c>
     </row>
@@ -11543,9 +11519,9 @@
   <dimension ref="A1:BL13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A6"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -12423,7 +12399,7 @@
       <c r="I6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K6" s="32" t="s">
@@ -12641,10 +12617,10 @@
       <c r="AE7" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AF7" s="75" t="s">
+      <c r="AF7" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="AG7" s="75" t="s">
+      <c r="AG7" s="70" t="s">
         <v>60</v>
       </c>
       <c r="AH7" s="7" t="s">
@@ -12799,10 +12775,10 @@
       <c r="AE8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AF8" s="75" t="s">
+      <c r="AF8" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="AG8" s="75" t="s">
+      <c r="AG8" s="70" t="s">
         <v>63</v>
       </c>
       <c r="AH8" s="7" t="s">
@@ -12967,10 +12943,10 @@
       <c r="AE9" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="AF9" s="75" t="s">
+      <c r="AF9" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="AG9" s="75" t="s">
+      <c r="AG9" s="70" t="s">
         <v>66</v>
       </c>
       <c r="AH9" s="7" t="s">
@@ -13093,7 +13069,7 @@
       <c r="I10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K10" s="32" t="s">
@@ -13157,10 +13133,10 @@
       <c r="AE10" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="AF10" s="75" t="s">
+      <c r="AF10" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="AG10" s="75" t="s">
+      <c r="AG10" s="70" t="s">
         <v>69</v>
       </c>
       <c r="AH10" s="7" t="s">
@@ -13275,7 +13251,7 @@
       <c r="I11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K11" s="32" t="s">
@@ -13453,7 +13429,7 @@
       <c r="I12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K12" s="32" t="s">
@@ -13631,7 +13607,7 @@
       <c r="I13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="75" t="s">
+      <c r="J13" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K13" s="32" t="s">
@@ -20142,7 +20118,7 @@
       <c r="I6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J6" s="75" t="s">
+      <c r="J6" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K6" s="32" t="s">
@@ -20273,7 +20249,7 @@
         <f t="shared" si="4"/>
         <v>VNPAY</v>
       </c>
-      <c r="BF6" s="75" t="str">
+      <c r="BF6" s="70" t="str">
         <f t="shared" si="5"/>
         <v>0355653300</v>
       </c>
@@ -20408,7 +20384,7 @@
       <c r="DA6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="DB6" s="75" t="s">
+      <c r="DB6" s="70" t="s">
         <v>168</v>
       </c>
       <c r="DC6" s="32" t="s">
@@ -20534,7 +20510,7 @@
       <c r="EW6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="EX6" s="75" t="s">
+      <c r="EX6" s="70" t="s">
         <v>168</v>
       </c>
       <c r="EY6" s="32" t="s">
@@ -20839,10 +20815,10 @@
       <c r="AE7" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AF7" s="75" t="s">
+      <c r="AF7" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="AG7" s="75" t="s">
+      <c r="AG7" s="70" t="s">
         <v>60</v>
       </c>
       <c r="AH7" s="7" t="s">
@@ -21404,10 +21380,10 @@
       <c r="AE8" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AF8" s="75" t="s">
+      <c r="AF8" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="AG8" s="75" t="s">
+      <c r="AG8" s="70" t="s">
         <v>63</v>
       </c>
       <c r="AH8" s="7" t="s">
@@ -22009,10 +21985,10 @@
       <c r="AE9" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="AF9" s="75" t="s">
+      <c r="AF9" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="AG9" s="75" t="s">
+      <c r="AG9" s="70" t="s">
         <v>66</v>
       </c>
       <c r="AH9" s="7" t="s">
@@ -22566,7 +22542,7 @@
       <c r="I10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J10" s="75" t="s">
+      <c r="J10" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K10" s="32" t="s">
@@ -22630,10 +22606,10 @@
       <c r="AE10" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="AF10" s="75" t="s">
+      <c r="AF10" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="AG10" s="75" t="s">
+      <c r="AG10" s="70" t="s">
         <v>69</v>
       </c>
       <c r="AH10" s="7" t="s">
@@ -22701,7 +22677,7 @@
         <f t="shared" si="4"/>
         <v>VNPAY</v>
       </c>
-      <c r="BF10" s="75" t="str">
+      <c r="BF10" s="70" t="str">
         <f t="shared" si="5"/>
         <v>0355653300</v>
       </c>
@@ -22836,7 +22812,7 @@
       <c r="DA10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="DB10" s="75" t="s">
+      <c r="DB10" s="70" t="s">
         <v>168</v>
       </c>
       <c r="DC10" s="32" t="s">
@@ -22962,7 +22938,7 @@
       <c r="EW10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="EX10" s="75" t="s">
+      <c r="EX10" s="70" t="s">
         <v>168</v>
       </c>
       <c r="EY10" s="32" t="s">
@@ -23227,7 +23203,7 @@
       <c r="I11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J11" s="75" t="s">
+      <c r="J11" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K11" s="32" t="s">
@@ -23358,7 +23334,7 @@
         <f t="shared" si="4"/>
         <v>VNPAY</v>
       </c>
-      <c r="BF11" s="75" t="str">
+      <c r="BF11" s="70" t="str">
         <f t="shared" si="5"/>
         <v>0355653300</v>
       </c>
@@ -23493,7 +23469,7 @@
       <c r="DA11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="DB11" s="75" t="s">
+      <c r="DB11" s="70" t="s">
         <v>168</v>
       </c>
       <c r="DC11" s="32" t="s">
@@ -23619,7 +23595,7 @@
       <c r="EW11" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="EX11" s="75" t="s">
+      <c r="EX11" s="70" t="s">
         <v>168</v>
       </c>
       <c r="EY11" s="32" t="s">
@@ -23884,7 +23860,7 @@
       <c r="I12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J12" s="75" t="s">
+      <c r="J12" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K12" s="32" t="s">
@@ -24015,7 +23991,7 @@
         <f t="shared" si="4"/>
         <v>VNPAY</v>
       </c>
-      <c r="BF12" s="75" t="str">
+      <c r="BF12" s="70" t="str">
         <f t="shared" si="5"/>
         <v>0355653300</v>
       </c>
@@ -24150,7 +24126,7 @@
       <c r="DA12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="DB12" s="75" t="s">
+      <c r="DB12" s="70" t="s">
         <v>168</v>
       </c>
       <c r="DC12" s="32" t="s">
@@ -24276,7 +24252,7 @@
       <c r="EW12" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="EX12" s="75" t="s">
+      <c r="EX12" s="70" t="s">
         <v>168</v>
       </c>
       <c r="EY12" s="32" t="s">
@@ -24541,7 +24517,7 @@
       <c r="I13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="75" t="s">
+      <c r="J13" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K13" s="32" t="s">
@@ -24672,7 +24648,7 @@
         <f t="shared" si="4"/>
         <v>VNPAY</v>
       </c>
-      <c r="BF13" s="75" t="str">
+      <c r="BF13" s="70" t="str">
         <f t="shared" si="5"/>
         <v>0355653300</v>
       </c>
@@ -24807,7 +24783,7 @@
       <c r="DA13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="DB13" s="75" t="s">
+      <c r="DB13" s="70" t="s">
         <v>168</v>
       </c>
       <c r="DC13" s="32" t="s">
@@ -24933,7 +24909,7 @@
       <c r="EW13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="EX13" s="75" t="s">
+      <c r="EX13" s="70" t="s">
         <v>168</v>
       </c>
       <c r="EY13" s="32" t="s">
@@ -25199,8 +25175,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
@@ -25600,8 +25576,8 @@
   <sheetPr/>
   <dimension ref="A1:BG10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1"/>
@@ -25609,7 +25585,7 @@
     <col min="1" max="1" width="13.7142857142857" style="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.952380952381" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1428571428571" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" customWidth="1"/>
     <col min="5" max="15" width="17.8380952380952" style="1" customWidth="1"/>
     <col min="16" max="16" width="17.8380952380952" style="28" customWidth="1"/>
     <col min="17" max="47" width="17.8380952380952" style="1" customWidth="1"/>
@@ -26014,10 +25990,10 @@
       <c r="Z3" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AA3" s="75" t="s">
+      <c r="AA3" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="75" t="s">
+      <c r="AB3" s="70" t="s">
         <v>60</v>
       </c>
       <c r="AC3" s="7" t="s">
@@ -26326,10 +26302,10 @@
       <c r="Z5" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="AA5" s="75" t="s">
+      <c r="AA5" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="AB5" s="75" t="s">
+      <c r="AB5" s="70" t="s">
         <v>63</v>
       </c>
       <c r="AC5" s="7" t="s">
@@ -26662,10 +26638,10 @@
       <c r="Z7" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="AA7" s="75" t="s">
+      <c r="AA7" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="AB7" s="75" t="s">
+      <c r="AB7" s="70" t="s">
         <v>66</v>
       </c>
       <c r="AC7" s="7" t="s">
@@ -26784,7 +26760,7 @@
       <c r="I8" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K8" s="32" t="s">
@@ -26943,7 +26919,7 @@
       <c r="I9" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="J9" s="75" t="s">
+      <c r="J9" s="70" t="s">
         <v>168</v>
       </c>
       <c r="K9" s="32" t="s">
@@ -26992,10 +26968,10 @@
       <c r="Z9" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="AA9" s="75" t="s">
+      <c r="AA9" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="AB9" s="75" t="s">
+      <c r="AB9" s="70" t="s">
         <v>69</v>
       </c>
       <c r="AC9" s="7" t="s">

</xml_diff>